<commit_message>
Personalities data with top3 artists information
</commit_message>
<xml_diff>
--- a/Output dataset/HoroscopCaracteristicsData.xlsx
+++ b/Output dataset/HoroscopCaracteristicsData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="2260" yWindow="700" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="183">
   <si>
     <t>Horoscopes</t>
   </si>
@@ -212,13 +212,370 @@
   </si>
   <si>
     <t>Edward Eldon Deane</t>
+  </si>
+  <si>
+    <t>Albers, Josef</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>Bottrop (M�_nster district, North Rhine-Westphalia, Germany)</t>
+  </si>
+  <si>
+    <t>Portfolio I, Folder 23</t>
+  </si>
+  <si>
+    <t>Lee, Edward B.</t>
+  </si>
+  <si>
+    <t>Sunrise 6:35 AM, Greenville, PA</t>
+  </si>
+  <si>
+    <t>Cole, Timothy|Century Company</t>
+  </si>
+  <si>
+    <t>American|American</t>
+  </si>
+  <si>
+    <t>London (Greater London, England, United Kingdom)|</t>
+  </si>
+  <si>
+    <t>Madonna and Child, by Giovanni Bellini</t>
+  </si>
+  <si>
+    <t>Hancock, John</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Untitled (Buttercup, JH 4)</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=111136&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Munhall, Walter</t>
+  </si>
+  <si>
+    <t>Construction workers riveting a truss</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=38731&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Douden, Herbert C.</t>
+  </si>
+  <si>
+    <t>Walls; [interior elevations]</t>
+  </si>
+  <si>
+    <t>Swank, Luke</t>
+  </si>
+  <si>
+    <t>Johnstown, PA</t>
+  </si>
+  <si>
+    <t>(Fair)</t>
+  </si>
+  <si>
+    <t>Goya, Francisco de</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Fuendetodos (Zaragoza province, Aragon, Spain)</t>
+  </si>
+  <si>
+    <t>Aquellos polbos. (Those Specks of Dust.)</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=94136&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Jorn, Asger</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>�rhus county (Denmark)</t>
+  </si>
+  <si>
+    <t>Semantic Virility</t>
+  </si>
+  <si>
+    <t>Mills, Frederick P.</t>
+  </si>
+  <si>
+    <t>Ceiling; [ornament drawings]</t>
+  </si>
+  <si>
+    <t>Hare, Clyde</t>
+  </si>
+  <si>
+    <t>Bloomington, Indiana</t>
+  </si>
+  <si>
+    <t>Automobiles on Liberty Bridge</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=9880&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Alechinsky, Pierre</t>
+  </si>
+  <si>
+    <t>Belgian</t>
+  </si>
+  <si>
+    <t>Brussels, Belgium</t>
+  </si>
+  <si>
+    <t>Lino-Litho</t>
+  </si>
+  <si>
+    <t>Spruance, Benton M.</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>Remainders</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=126459&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Bochner, Mel</t>
+  </si>
+  <si>
+    <t>Pittsburgh, Pennsylvania</t>
+  </si>
+  <si>
+    <t>Design for Kraus Campo, Carnegie Mellon University: Study for"You Can Call it That if You Like"</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=133238&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Callot, Jacques</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Nancy (Meurthe-et-Moselle, Lorraine, France)</t>
+  </si>
+  <si>
+    <t>Drill with the Musket</t>
+  </si>
+  <si>
+    <t>Kauffman, William</t>
+  </si>
+  <si>
+    <t>Courthouse; Westmoreland County Courthouse, Greensburg, PA; [detail drawings, plan]</t>
+  </si>
+  <si>
+    <t>Hood, Samuel S.</t>
+  </si>
+  <si>
+    <t>Leonard Lieb (Face)</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=111697&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Lefebre, John</t>
+  </si>
+  <si>
+    <t>Berlin, Germany</t>
+  </si>
+  <si>
+    <t>Asger Jorn (Albisola, 1955)</t>
+  </si>
+  <si>
+    <t>Smith, W. Eugene</t>
+  </si>
+  <si>
+    <t>Wichita, Kansas</t>
+  </si>
+  <si>
+    <t>City Council Chamber, City Council Building</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=28980&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Whistler, James McNeill</t>
+  </si>
+  <si>
+    <t>Lowell, Massachusetts</t>
+  </si>
+  <si>
+    <t>The Little Nude Model, Reading</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=56834&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Rijn, Rembrandt H. Van</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Netherlands, Leyden</t>
+  </si>
+  <si>
+    <t>Saints Peter and John Healing the Cripple at the Gate of the Temple</t>
+  </si>
+  <si>
+    <t>Ruzicka, Rudolph</t>
+  </si>
+  <si>
+    <t>Bohemia (Czech Republic)</t>
+  </si>
+  <si>
+    <t>The Washington Monument in the Public Garden, Boston</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=100978&amp;size=Medium|http://www.cmoa.org/CollectionImage.aspx?irn=100979&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Rouault, Georges</t>
+  </si>
+  <si>
+    <t>Paris, France</t>
+  </si>
+  <si>
+    <t>Woman with Necklace</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=124800&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Hassam, Childe</t>
+  </si>
+  <si>
+    <t>Dorchester (Suffolk county, Massachusetts, United States)</t>
+  </si>
+  <si>
+    <t>Old Mulford House</t>
+  </si>
+  <si>
+    <t>Rosenberg, Samuel</t>
+  </si>
+  <si>
+    <t>Philadelphia (Philadelphia county, Pennsylvania, United States)</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Leopold, Otto Gerhard</t>
+  </si>
+  <si>
+    <t>Germany (Europe)</t>
+  </si>
+  <si>
+    <t>Cook, Robert A.</t>
+  </si>
+  <si>
+    <t>School; [floor plan] (en suite with 1997.29.34.1-.5)</t>
+  </si>
+  <si>
+    <t>Biddle, George</t>
+  </si>
+  <si>
+    <t>Adam and Eve</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=100726&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Saint, Lawrence B.</t>
+  </si>
+  <si>
+    <t>Sharpsburgh, Pennsylvania</t>
+  </si>
+  <si>
+    <t>Drapery from a Sleeve of the Virgin, Window at West End of Church of St. Vincent, Rouen</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=106095&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Johnston, Ralph W.</t>
+  </si>
+  <si>
+    <t>(Carnegie Library of Pittsburgh: Home Library Girl's Club, February 7, 1907)</t>
+  </si>
+  <si>
+    <t>Strauss, Zoe</t>
+  </si>
+  <si>
+    <t>Philadelphia, Pennsylvania, United States of America</t>
+  </si>
+  <si>
+    <t>Homesteading</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=130922&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Mellan, Claude</t>
+  </si>
+  <si>
+    <t>Abbeville, France</t>
+  </si>
+  <si>
+    <t>Antique Statue: Young Man</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=105517&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Mauve, Anton</t>
+  </si>
+  <si>
+    <t>Zaandam, North Holland, Netherlands</t>
+  </si>
+  <si>
+    <t>Wood Choppers</t>
+  </si>
+  <si>
+    <t>Bendiner, Alfred</t>
+  </si>
+  <si>
+    <t>Travel is so Broadening</t>
+  </si>
+  <si>
+    <t>http://www.cmoa.org/CollectionImage.aspx?irn=89492&amp;size=Medium|http://www.cmoa.org/CollectionImage.aspx?irn=47103&amp;size=Medium</t>
+  </si>
+  <si>
+    <t>Walfish, Herbert S.</t>
+  </si>
+  <si>
+    <t>School; [exterior perspective] (en suite with 95.127.16-.22)</t>
+  </si>
+  <si>
+    <t>Deane, Edward E.</t>
+  </si>
+  <si>
+    <t>Untitled (Man), from Sketchbook (en suite with 91.23.12.1-.15)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +595,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,8 +633,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -608,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -619,7 +984,7 @@
     <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -693,100 +1058,762 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2">
+        <v>1888</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2">
+        <v>72</v>
+      </c>
+      <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2">
+        <v>1876</v>
+      </c>
+      <c r="S2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2">
+        <v>63</v>
+      </c>
+      <c r="W2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2">
+        <v>1852</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3">
+        <v>1757</v>
+      </c>
+      <c r="K3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3">
+        <v>58</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3">
+        <v>1901</v>
+      </c>
+      <c r="S3" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" t="s">
+        <v>81</v>
+      </c>
+      <c r="U3" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3">
+        <v>42</v>
+      </c>
+      <c r="W3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3">
+        <v>1901</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4">
+        <v>338</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4">
+        <v>1890</v>
+      </c>
+      <c r="K4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O4">
+        <v>105</v>
+      </c>
+      <c r="P4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q4">
+        <v>1746</v>
+      </c>
+      <c r="R4" t="s">
+        <v>89</v>
+      </c>
+      <c r="S4" t="s">
+        <v>90</v>
+      </c>
+      <c r="T4" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" t="s">
+        <v>92</v>
+      </c>
+      <c r="V4">
+        <v>32</v>
+      </c>
+      <c r="W4" t="s">
+        <v>93</v>
+      </c>
+      <c r="X4">
+        <v>1914</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="G5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="1">
+        <v>224</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1879</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" s="1">
+        <v>142</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1927</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V5" s="1">
+        <v>101</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1927</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="G6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="1">
+        <v>128</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1904</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="1">
+        <v>70</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1940</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="V6" s="1">
+        <v>63</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1592</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7">
+        <v>1857</v>
+      </c>
+      <c r="L7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N7" t="s">
+        <v>120</v>
+      </c>
+      <c r="O7">
+        <v>85</v>
+      </c>
+      <c r="P7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7">
+        <v>1917</v>
+      </c>
+      <c r="S7" t="s">
+        <v>121</v>
+      </c>
+      <c r="T7" t="s">
+        <v>122</v>
+      </c>
+      <c r="U7" t="s">
+        <v>123</v>
+      </c>
+      <c r="V7">
+        <v>77</v>
+      </c>
+      <c r="W7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7">
+        <v>1905</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8">
+        <v>571</v>
+      </c>
+      <c r="I8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8">
+        <v>1918</v>
+      </c>
+      <c r="K8" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" t="s">
+        <v>128</v>
+      </c>
+      <c r="M8" t="s">
+        <v>129</v>
+      </c>
+      <c r="N8" t="s">
+        <v>130</v>
+      </c>
+      <c r="O8">
+        <v>125</v>
+      </c>
+      <c r="P8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8">
+        <v>1834</v>
+      </c>
+      <c r="R8" t="s">
+        <v>131</v>
+      </c>
+      <c r="S8" t="s">
+        <v>132</v>
+      </c>
+      <c r="T8" t="s">
+        <v>133</v>
+      </c>
+      <c r="U8" t="s">
+        <v>134</v>
+      </c>
+      <c r="V8">
+        <v>64</v>
+      </c>
+      <c r="W8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X8">
+        <v>1606</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="G9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9">
+        <v>95</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9">
+        <v>1883</v>
+      </c>
+      <c r="K9" t="s">
+        <v>139</v>
+      </c>
+      <c r="L9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" t="s">
+        <v>141</v>
+      </c>
+      <c r="N9" t="s">
+        <v>142</v>
+      </c>
+      <c r="O9">
+        <v>88</v>
+      </c>
+      <c r="P9" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q9">
+        <v>1871</v>
+      </c>
+      <c r="R9" t="s">
+        <v>143</v>
+      </c>
+      <c r="S9" t="s">
+        <v>144</v>
+      </c>
+      <c r="T9" t="s">
+        <v>145</v>
+      </c>
+      <c r="U9" t="s">
+        <v>146</v>
+      </c>
+      <c r="V9">
+        <v>83</v>
+      </c>
+      <c r="W9" t="s">
+        <v>65</v>
+      </c>
+      <c r="X9">
+        <v>1859</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="G10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10">
+        <v>626</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10">
+        <v>1896</v>
+      </c>
+      <c r="K10" t="s">
+        <v>150</v>
+      </c>
+      <c r="L10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O10">
+        <v>203</v>
+      </c>
+      <c r="P10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q10">
+        <v>1824</v>
+      </c>
+      <c r="R10" t="s">
+        <v>153</v>
+      </c>
+      <c r="U10" t="s">
+        <v>154</v>
+      </c>
+      <c r="V10">
+        <v>141</v>
+      </c>
+      <c r="W10" t="s">
+        <v>65</v>
+      </c>
+      <c r="X10">
+        <v>1872</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="G11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H11">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11">
+        <v>1885</v>
+      </c>
+      <c r="L11" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" t="s">
+        <v>158</v>
+      </c>
+      <c r="N11" t="s">
+        <v>159</v>
+      </c>
+      <c r="O11">
+        <v>81</v>
+      </c>
+      <c r="P11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q11">
+        <v>1885</v>
+      </c>
+      <c r="R11" t="s">
+        <v>160</v>
+      </c>
+      <c r="S11" t="s">
+        <v>161</v>
+      </c>
+      <c r="T11" t="s">
+        <v>162</v>
+      </c>
+      <c r="U11" t="s">
+        <v>163</v>
+      </c>
+      <c r="V11">
+        <v>57</v>
+      </c>
+      <c r="W11" t="s">
+        <v>65</v>
+      </c>
+      <c r="X11">
+        <v>1873</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="G12" t="s">
+        <v>165</v>
+      </c>
+      <c r="H12">
+        <v>221</v>
+      </c>
+      <c r="I12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12">
+        <v>1970</v>
+      </c>
+      <c r="K12" t="s">
+        <v>166</v>
+      </c>
+      <c r="L12" t="s">
+        <v>167</v>
+      </c>
+      <c r="M12" t="s">
+        <v>168</v>
+      </c>
+      <c r="N12" t="s">
+        <v>169</v>
+      </c>
+      <c r="O12">
+        <v>120</v>
+      </c>
+      <c r="P12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12">
+        <v>1598</v>
+      </c>
+      <c r="R12" t="s">
+        <v>170</v>
+      </c>
+      <c r="S12" t="s">
+        <v>171</v>
+      </c>
+      <c r="T12" t="s">
+        <v>172</v>
+      </c>
+      <c r="U12" t="s">
+        <v>173</v>
+      </c>
+      <c r="V12">
+        <v>47</v>
+      </c>
+      <c r="W12" t="s">
+        <v>135</v>
+      </c>
+      <c r="X12">
+        <v>1838</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13">
+        <v>77</v>
+      </c>
+      <c r="I13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13">
+        <v>1899</v>
+      </c>
+      <c r="K13" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" t="s">
+        <v>177</v>
+      </c>
+      <c r="M13" t="s">
+        <v>178</v>
+      </c>
+      <c r="N13" t="s">
+        <v>179</v>
+      </c>
+      <c r="O13">
+        <v>73</v>
+      </c>
+      <c r="P13" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q13">
+        <v>1923</v>
+      </c>
+      <c r="S13" t="s">
+        <v>180</v>
+      </c>
+      <c r="U13" t="s">
+        <v>181</v>
+      </c>
+      <c r="V13">
+        <v>54</v>
+      </c>
+      <c r="W13" t="s">
+        <v>75</v>
+      </c>
+      <c r="X13">
+        <v>1851</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>